<commit_message>
- Captura datos (Hoteles, Vuelos y Asistencias)
</commit_message>
<xml_diff>
--- a/app/prueba_carga.xlsx
+++ b/app/prueba_carga.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="ON" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OFF" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ON" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="OFF" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="184">
   <si>
     <t xml:space="preserve">Owner</t>
   </si>
@@ -793,284 +793,280 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1146,18 +1142,124 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:CG7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AU1" activeCellId="0" sqref="AU1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AR1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AY33" activeCellId="0" sqref="AY33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.72"/>
@@ -1182,19 +1284,19 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="11.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="2" width="13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="13.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="1" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="2" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="13.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="9.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="2" width="14.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="13.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="4" width="11.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="2" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="4" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="4" width="17.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="16.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="12.72"/>
@@ -2088,11 +2190,19 @@
       <c r="AQ5" s="31"/>
       <c r="AR5" s="31"/>
       <c r="AS5" s="37"/>
-      <c r="AT5" s="31"/>
-      <c r="AU5" s="41"/>
-      <c r="AV5" s="41"/>
+      <c r="AT5" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU5" s="34" t="n">
+        <v>45558</v>
+      </c>
+      <c r="AV5" s="34" t="n">
+        <v>45559</v>
+      </c>
       <c r="AW5" s="31"/>
-      <c r="AX5" s="31"/>
+      <c r="AX5" s="39" t="s">
+        <v>117</v>
+      </c>
       <c r="AY5" s="31"/>
       <c r="AZ5" s="41"/>
       <c r="BA5" s="41"/>
@@ -2177,11 +2287,19 @@
       <c r="AQ6" s="31"/>
       <c r="AR6" s="31"/>
       <c r="AS6" s="37"/>
-      <c r="AT6" s="31"/>
-      <c r="AU6" s="41"/>
-      <c r="AV6" s="41"/>
-      <c r="AW6" s="31"/>
-      <c r="AX6" s="31"/>
+      <c r="AT6" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU6" s="34" t="n">
+        <v>45558</v>
+      </c>
+      <c r="AV6" s="34" t="n">
+        <v>45559</v>
+      </c>
+      <c r="AW6" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="AX6" s="39"/>
       <c r="AY6" s="31"/>
       <c r="AZ6" s="41"/>
       <c r="BA6" s="41"/>
@@ -2220,7 +2338,18 @@
       <c r="CF6" s="41"/>
       <c r="CG6" s="31"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AT7" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="AU7" s="34" t="n">
+        <v>45558</v>
+      </c>
+      <c r="AV7" s="34" t="n">
+        <v>45559</v>
+      </c>
+      <c r="AW7" s="31"/>
+      <c r="AX7" s="39"/>
       <c r="BF7" s="47"/>
     </row>
   </sheetData>
@@ -2235,17 +2364,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BV4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AT3" activeCellId="0" sqref="AT3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.15"/>
@@ -2257,7 +2386,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="26.15"/>
@@ -2270,7 +2399,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="48" width="12.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="48" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="49" width="17.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="48" width="17.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="48" width="17.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="48" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="50" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="51" width="11.72"/>
@@ -2740,7 +2869,7 @@
       <c r="AF3" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="AG3" s="64" t="n">
+      <c r="AG3" s="31" t="n">
         <v>2</v>
       </c>
       <c r="AH3" s="31" t="s">
@@ -2912,10 +3041,10 @@
       <c r="P4" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
       <c r="U4" s="31" t="s">
         <v>178</v>
       </c>
@@ -2934,51 +3063,51 @@
       <c r="Z4" s="31" t="s">
         <v>183</v>
       </c>
-      <c r="AA4" s="65"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="65"/>
-      <c r="AE4" s="65"/>
-      <c r="AF4" s="65"/>
-      <c r="AG4" s="68"/>
-      <c r="AH4" s="65"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="68"/>
-      <c r="AK4" s="65"/>
-      <c r="AL4" s="65"/>
-      <c r="AM4" s="65"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="65"/>
-      <c r="AQ4" s="65"/>
-      <c r="AR4" s="65"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="69"/>
-      <c r="AU4" s="65"/>
-      <c r="AV4" s="65"/>
-      <c r="AW4" s="65"/>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="65"/>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="65"/>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="65"/>
-      <c r="BD4" s="69"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
+      <c r="AM4" s="64"/>
+      <c r="AN4" s="65"/>
+      <c r="AO4" s="65"/>
+      <c r="AP4" s="64"/>
+      <c r="AQ4" s="64"/>
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="65"/>
+      <c r="AT4" s="68"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="64"/>
+      <c r="AX4" s="66"/>
+      <c r="AY4" s="64"/>
+      <c r="AZ4" s="67"/>
+      <c r="BA4" s="64"/>
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="64"/>
+      <c r="BD4" s="68"/>
       <c r="BE4" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="BF4" s="65"/>
-      <c r="BG4" s="65"/>
-      <c r="BH4" s="65"/>
-      <c r="BI4" s="65"/>
-      <c r="BJ4" s="65"/>
-      <c r="BK4" s="65"/>
-      <c r="BL4" s="65"/>
-      <c r="BM4" s="65"/>
-      <c r="BN4" s="65"/>
-      <c r="BO4" s="65"/>
-      <c r="BP4" s="65"/>
-      <c r="BQ4" s="65"/>
+      <c r="BF4" s="64"/>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="64"/>
+      <c r="BJ4" s="64"/>
+      <c r="BK4" s="64"/>
+      <c r="BL4" s="64"/>
+      <c r="BM4" s="64"/>
+      <c r="BN4" s="64"/>
+      <c r="BO4" s="64"/>
+      <c r="BP4" s="64"/>
+      <c r="BQ4" s="64"/>
       <c r="BR4" s="31"/>
       <c r="BS4" s="31"/>
       <c r="BT4" s="31" t="s">

</xml_diff>

<commit_message>
Carga de todos los datos
</commit_message>
<xml_diff>
--- a/app/prueba_carga.xlsx
+++ b/app/prueba_carga.xlsx
@@ -8,8 +8,8 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="ON" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="OFF" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ON" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="OFF" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="186">
   <si>
     <t xml:space="preserve">Owner</t>
   </si>
@@ -503,6 +503,12 @@
     <t xml:space="preserve">II1265345F</t>
   </si>
   <si>
+    <t xml:space="preserve">LA88 PUQ SCL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3:26+1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tripulante</t>
   </si>
   <si>
@@ -512,6 +518,9 @@
     <t xml:space="preserve">Zhou</t>
   </si>
   <si>
+    <t xml:space="preserve">15/03/24</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hotel SCL</t>
   </si>
   <si>
@@ -558,9 +567,6 @@
   </si>
   <si>
     <t xml:space="preserve">KL702 SCL AMS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26-10-2023</t>
   </si>
   <si>
     <t xml:space="preserve">10:50 - 12:00</t>
@@ -579,7 +585,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="10">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="#,##0"/>
@@ -589,6 +595,7 @@
     <numFmt numFmtId="170" formatCode="dd/mm/yy\ h:mm"/>
     <numFmt numFmtId="171" formatCode="d/m/yy"/>
     <numFmt numFmtId="172" formatCode="#,##0.00"/>
+    <numFmt numFmtId="173" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -793,284 +800,280 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="171" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="173" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1146,8 +1149,114 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1157,12 +1266,12 @@
       <selection pane="topLeft" activeCell="AU1" activeCellId="0" sqref="AU1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="10.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="15.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.86"/>
@@ -1170,7 +1279,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="10.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="10.29"/>
@@ -1217,13 +1326,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="2" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="2" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="13.72"/>
@@ -1231,11 +1340,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="72" min="72" style="1" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="73" min="73" style="1" width="9.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="1" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="75" min="75" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="76" min="76" style="1" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="77" min="77" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="78" min="78" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="1" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="79" min="79" style="1" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="80" min="80" style="1" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="81" min="81" style="1" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="82" min="82" style="1" width="12.57"/>
@@ -2235,17 +2344,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:BV4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AB1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AT3" activeCellId="0" sqref="AT3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V2" activeCellId="0" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.15"/>
@@ -2258,9 +2367,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="9.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="26.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="2" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="48" width="13"/>
@@ -2293,13 +2402,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="52" width="9.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="48" width="7.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="48" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="48" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="48" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="51" width="8.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="48" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="48" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="49" width="8.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="48" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="48" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="51" width="8.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="48" width="10.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="48" width="10.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="52" width="8.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="1" width="13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="48" width="13.72"/>
@@ -2307,11 +2416,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="48" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="48" width="9.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="48" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="48" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="63" style="48" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="48" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="48" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="48" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="48" width="11.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="48" width="11.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="48" width="11.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="48" width="10.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="12.57"/>
@@ -2598,15 +2707,21 @@
       <c r="R2" s="31"/>
       <c r="S2" s="31"/>
       <c r="T2" s="31"/>
-      <c r="U2" s="31"/>
-      <c r="V2" s="31"/>
-      <c r="W2" s="31"/>
+      <c r="U2" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="V2" s="61" t="n">
+        <v>45637</v>
+      </c>
+      <c r="W2" s="31" t="s">
+        <v>161</v>
+      </c>
       <c r="X2" s="31"/>
       <c r="Y2" s="41"/>
       <c r="Z2" s="31"/>
       <c r="AA2" s="31"/>
       <c r="AB2" s="37"/>
-      <c r="AC2" s="61"/>
+      <c r="AC2" s="62"/>
       <c r="AD2" s="31"/>
       <c r="AE2" s="31"/>
       <c r="AF2" s="31"/>
@@ -2627,11 +2742,11 @@
       <c r="AU2" s="31"/>
       <c r="AV2" s="31"/>
       <c r="AW2" s="31"/>
-      <c r="AX2" s="62"/>
+      <c r="AX2" s="63"/>
       <c r="AY2" s="42"/>
       <c r="AZ2" s="41"/>
       <c r="BA2" s="31"/>
-      <c r="BB2" s="61"/>
+      <c r="BB2" s="62"/>
       <c r="BC2" s="39"/>
       <c r="BD2" s="38"/>
       <c r="BE2" s="31"/>
@@ -2673,7 +2788,7 @@
         <v>98</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H3" s="31" t="s">
         <v>100</v>
@@ -2682,10 +2797,10 @@
         <v>100</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="K3" s="31" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="L3" s="31" t="s">
         <v>90</v>
@@ -2711,11 +2826,13 @@
       <c r="U3" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="V3" s="31"/>
+      <c r="V3" s="31" t="s">
+        <v>165</v>
+      </c>
       <c r="W3" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="X3" s="63"/>
+      <c r="X3" s="31"/>
       <c r="Y3" s="34" t="n">
         <v>45218</v>
       </c>
@@ -2728,7 +2845,7 @@
       <c r="AB3" s="37" t="n">
         <v>45577</v>
       </c>
-      <c r="AC3" s="61" t="n">
+      <c r="AC3" s="62" t="n">
         <v>0.958333333333333</v>
       </c>
       <c r="AD3" s="31" t="s">
@@ -2740,11 +2857,11 @@
       <c r="AF3" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="AG3" s="64" t="n">
+      <c r="AG3" s="31" t="n">
         <v>2</v>
       </c>
       <c r="AH3" s="31" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="AI3" s="36" t="n">
         <v>45554</v>
@@ -2756,10 +2873,10 @@
         <v>116</v>
       </c>
       <c r="AL3" s="31" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="AM3" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AN3" s="34" t="n">
         <v>45555</v>
@@ -2771,10 +2888,10 @@
         <v>116</v>
       </c>
       <c r="AQ3" s="31" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="AR3" s="31" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="AS3" s="34" t="n">
         <v>45558</v>
@@ -2786,12 +2903,12 @@
         <v>116</v>
       </c>
       <c r="AV3" s="31" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AW3" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="AX3" s="62" t="n">
+      <c r="AX3" s="63" t="n">
         <v>45562.75</v>
       </c>
       <c r="AY3" s="42" t="s">
@@ -2803,7 +2920,7 @@
       <c r="BA3" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="BB3" s="61" t="n">
+      <c r="BB3" s="62" t="n">
         <v>45562.75</v>
       </c>
       <c r="BC3" s="39" t="s">
@@ -2852,10 +2969,10 @@
         <v>122</v>
       </c>
       <c r="BR3" s="31" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="BS3" s="31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="BT3" s="31" t="s">
         <v>124</v>
@@ -2887,98 +3004,98 @@
         <v>87</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H4" s="31"/>
       <c r="I4" s="31"/>
       <c r="J4" s="31" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="L4" s="31" t="s">
         <v>132</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="N4" s="31" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="O4" s="31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="P4" s="41" t="s">
-        <v>177</v>
-      </c>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
+        <v>180</v>
+      </c>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
       <c r="U4" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="V4" s="31" t="s">
-        <v>179</v>
+        <v>181</v>
+      </c>
+      <c r="V4" s="40" t="n">
+        <v>45225</v>
       </c>
       <c r="W4" s="31" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="X4" s="31" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="Y4" s="31" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="Z4" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA4" s="65"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="67"/>
-      <c r="AD4" s="65"/>
-      <c r="AE4" s="65"/>
-      <c r="AF4" s="65"/>
-      <c r="AG4" s="68"/>
-      <c r="AH4" s="65"/>
-      <c r="AI4" s="69"/>
-      <c r="AJ4" s="68"/>
-      <c r="AK4" s="65"/>
-      <c r="AL4" s="65"/>
-      <c r="AM4" s="65"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="65"/>
-      <c r="AQ4" s="65"/>
-      <c r="AR4" s="65"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="69"/>
-      <c r="AU4" s="65"/>
-      <c r="AV4" s="65"/>
-      <c r="AW4" s="65"/>
-      <c r="AX4" s="67"/>
-      <c r="AY4" s="65"/>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="65"/>
-      <c r="BB4" s="67"/>
-      <c r="BC4" s="65"/>
-      <c r="BD4" s="69"/>
+        <v>185</v>
+      </c>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="65"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="67"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="68"/>
+      <c r="AJ4" s="67"/>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
+      <c r="AM4" s="64"/>
+      <c r="AN4" s="65"/>
+      <c r="AO4" s="65"/>
+      <c r="AP4" s="64"/>
+      <c r="AQ4" s="64"/>
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="65"/>
+      <c r="AT4" s="68"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="64"/>
+      <c r="AX4" s="66"/>
+      <c r="AY4" s="64"/>
+      <c r="AZ4" s="67"/>
+      <c r="BA4" s="64"/>
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="64"/>
+      <c r="BD4" s="68"/>
       <c r="BE4" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="BF4" s="65"/>
-      <c r="BG4" s="65"/>
-      <c r="BH4" s="65"/>
-      <c r="BI4" s="65"/>
-      <c r="BJ4" s="65"/>
-      <c r="BK4" s="65"/>
-      <c r="BL4" s="65"/>
-      <c r="BM4" s="65"/>
-      <c r="BN4" s="65"/>
-      <c r="BO4" s="65"/>
-      <c r="BP4" s="65"/>
-      <c r="BQ4" s="65"/>
+      <c r="BF4" s="64"/>
+      <c r="BG4" s="64"/>
+      <c r="BH4" s="64"/>
+      <c r="BI4" s="64"/>
+      <c r="BJ4" s="64"/>
+      <c r="BK4" s="64"/>
+      <c r="BL4" s="64"/>
+      <c r="BM4" s="64"/>
+      <c r="BN4" s="64"/>
+      <c r="BO4" s="64"/>
+      <c r="BP4" s="64"/>
+      <c r="BQ4" s="64"/>
       <c r="BR4" s="31"/>
       <c r="BS4" s="31"/>
       <c r="BT4" s="31" t="s">

</xml_diff>